<commit_message>
Updated labelling code and labels (see note)
The version of 05-labelling/02-labelling.py used for labelling included a condition for (meanwj['Name'].isna()) in line 38. As such, for each feature, the code would return the top 20 unlabelled topics. This means that extra topics were labelled beyond the top 20 in each feature (since some topics appear in the true top 20 across several lists). The extra topic labels are preserved for transparency, but are not included in further analysis since they were dependent on the ordering of the features. The extra labels were identified by re-sorting the dataframe on each feature and collecting the topic IDs that did not appear in any of the top 20s.

All labels recorded in file: support_data/label agreement (extra labels).xlsx
Labels used for presentation and accuracy calculations going forward are in
file: support_data/label agreement.xlsx
</commit_message>
<xml_diff>
--- a/support_data/label agreement.xlsx
+++ b/support_data/label agreement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Patrick/Documents/OII/Project/Code/SC1/WikiNewsNetwork-01-WikiNewsTopics/support_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B995CA4E-9399-8D40-8FDC-2393D56C9BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C487DA-D2BC-8240-940D-1B83795A41B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-100" windowWidth="38400" windowHeight="21100" xr2:uid="{A0328CC9-6EC5-A44E-9BC3-3A8F26FE8663}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="20500" activeTab="1" xr2:uid="{A0328CC9-6EC5-A44E-9BC3-3A8F26FE8663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="134">
   <si>
     <t>Countries</t>
   </si>
@@ -152,12 +152,6 @@
     <t>Big Tech companies</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaza–Israel conflict </t>
-  </si>
-  <si>
-    <t>Gaza border protests</t>
-  </si>
-  <si>
     <t>Brett Kavanaugh Supreme Court nomination</t>
   </si>
   <si>
@@ -176,39 +170,18 @@
     <t>US mass shootings</t>
   </si>
   <si>
-    <t>(Neo)Nazism</t>
-  </si>
-  <si>
-    <t>Holocaust</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United kingdom </t>
-  </si>
-  <si>
     <t>Turkey–United States relations</t>
   </si>
   <si>
     <t>california wildfires</t>
   </si>
   <si>
-    <t>Naval accidents</t>
-  </si>
-  <si>
-    <t>shipwrecks</t>
-  </si>
-  <si>
     <t>Australian Politics</t>
   </si>
   <si>
     <t>Asia</t>
   </si>
   <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
     <t>US Finance</t>
   </si>
   <si>
@@ -227,12 +200,6 @@
     <t>Olympic games</t>
   </si>
   <si>
-    <t>Ethiopian Politics</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Puna eruption </t>
   </si>
   <si>
@@ -296,12 +263,6 @@
     <t>Tesla Inc.</t>
   </si>
   <si>
-    <t>Spanish Prime Ministers</t>
-  </si>
-  <si>
-    <t>Spanish politics</t>
-  </si>
-  <si>
     <t>Tennis</t>
   </si>
   <si>
@@ -311,21 +272,6 @@
     <t>Israel in Syrian civil war</t>
   </si>
   <si>
-    <t>MLB</t>
-  </si>
-  <si>
-    <t>Baseball</t>
-  </si>
-  <si>
-    <t>Johnson Family</t>
-  </si>
-  <si>
-    <t>Assassination of Jamal Khashoggi</t>
-  </si>
-  <si>
-    <t>Jamal Khashoggi</t>
-  </si>
-  <si>
     <t>US Gun violence</t>
   </si>
   <si>
@@ -344,27 +290,12 @@
     <t>Yemen</t>
   </si>
   <si>
-    <t>Lombok earthquake</t>
-  </si>
-  <si>
-    <t>Sri Lankan Politics</t>
-  </si>
-  <si>
-    <t>Sri Lankan politics 2018</t>
-  </si>
-  <si>
     <t>Russia-Ukraine relations</t>
   </si>
   <si>
     <t xml:space="preserve">Terrorism in Turkey </t>
   </si>
   <si>
-    <t>Indian Prime Ministers</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Australian Prime Ministers</t>
   </si>
   <si>
@@ -395,12 +326,6 @@
     <t>Costa Rica politics</t>
   </si>
   <si>
-    <t>NHL</t>
-  </si>
-  <si>
-    <t>National Hockey League</t>
-  </si>
-  <si>
     <t>Indian Politics</t>
   </si>
   <si>
@@ -431,9 +356,6 @@
     <t>Puna Volcano</t>
   </si>
   <si>
-    <t>Indonesia earthquake</t>
-  </si>
-  <si>
     <t>East Asia</t>
   </si>
   <si>
@@ -464,9 +386,6 @@
     <t>Israeli conflict</t>
   </si>
   <si>
-    <t>Boris Johnson Family</t>
-  </si>
-  <si>
     <t>Unanimous Strong</t>
   </si>
   <si>
@@ -510,12 +429,6 @@
   </si>
   <si>
     <t>US Domestic</t>
-  </si>
-  <si>
-    <t>Pakistani Politics 2</t>
-  </si>
-  <si>
-    <t>Pakistani Politics 1</t>
   </si>
   <si>
     <t>California Wildfires 2</t>
@@ -879,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7CE3DF-1B66-FD45-A1A9-D3B5D7DFE1DD}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,31 +806,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="I1" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -931,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F2">
         <f>COUNTIF(D2:E2, "S")</f>
@@ -964,25 +877,25 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">COUNTIF(D3:E3, "S")</f>
+        <f t="shared" ref="F3:F54" si="0">COUNTIF(D3:E3, "S")</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G66" si="1">COUNTIF(D3:E3, "P")</f>
+        <f t="shared" ref="G3:G54" si="1">COUNTIF(D3:E3, "P")</f>
         <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="2">COUNTIF(D3:E3, "N")</f>
+        <f t="shared" ref="H3:H54" si="2">COUNTIF(D3:E3, "N")</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="3">SUM(F3:H3)</f>
+        <f t="shared" ref="I3:I54" si="3">SUM(F3:H3)</f>
         <v>2</v>
       </c>
     </row>
@@ -991,16 +904,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -1030,10 +943,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -1063,10 +976,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -1096,10 +1009,10 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -1129,10 +1042,10 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -1162,10 +1075,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -1195,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -1228,10 +1141,10 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1261,10 +1174,10 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1294,10 +1207,10 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -1324,13 +1237,13 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -1360,10 +1273,10 @@
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -1387,16 +1300,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1426,10 +1339,10 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1456,13 +1369,13 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -1489,13 +1402,13 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1525,10 +1438,10 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -1558,10 +1471,10 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -1591,10 +1504,10 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1624,10 +1537,10 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1657,10 +1570,10 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
@@ -1690,10 +1603,10 @@
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
@@ -1714,7 +1627,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
@@ -1723,18 +1636,18 @@
         <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
@@ -1747,7 +1660,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
@@ -1756,18 +1669,18 @@
         <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
@@ -1780,7 +1693,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
@@ -1789,10 +1702,10 @@
         <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -1813,19 +1726,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -1846,27 +1759,27 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
         <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
@@ -1879,27 +1792,27 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
@@ -1912,23 +1825,23 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -1936,7 +1849,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
@@ -1945,19 +1858,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -1978,19 +1891,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
@@ -2011,27 +1924,27 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
@@ -2044,27 +1957,27 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
@@ -2077,19 +1990,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -2110,19 +2023,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
@@ -2143,19 +2056,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -2176,19 +2089,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
@@ -2209,27 +2122,27 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
@@ -2242,27 +2155,27 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E42" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
@@ -2275,23 +2188,23 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
         <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
@@ -2299,7 +2212,7 @@
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <f t="shared" si="3"/>
@@ -2308,19 +2221,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" t="s">
         <v>68</v>
       </c>
-      <c r="C44" t="s">
-        <v>69</v>
-      </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
@@ -2341,19 +2254,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
         <v>70</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E45" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
@@ -2374,7 +2287,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>148</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
         <v>71</v>
@@ -2383,10 +2296,10 @@
         <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E46" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
@@ -2407,7 +2320,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
         <v>73</v>
@@ -2416,18 +2329,18 @@
         <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E47" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
@@ -2440,7 +2353,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
         <v>75</v>
@@ -2449,10 +2362,10 @@
         <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
@@ -2473,27 +2386,27 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="B49" t="s">
         <v>77</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E49" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
@@ -2506,19 +2419,19 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E50" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
@@ -2539,19 +2452,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D51" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E51" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
@@ -2572,19 +2485,19 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E52" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
@@ -2605,19 +2518,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D53" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E53" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
@@ -2638,19 +2551,19 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>188</v>
+        <v>257</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E54" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
@@ -2671,891 +2584,396 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D55" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E55" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="F55:F66" si="4">COUNTIF(D55:E55, "S")</f>
+        <v>0</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="G55:G66" si="5">COUNTIF(D55:E55, "P")</f>
+        <v>2</v>
       </c>
       <c r="H55">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H55:H66" si="6">COUNTIF(D55:E55, "N")</f>
         <v>0</v>
       </c>
       <c r="I55">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I55:I66" si="7">SUM(F55:H55)</f>
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>207</v>
+        <v>307</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E56" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G56">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="H56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>242</v>
+        <v>310</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>240</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" t="s">
         <v>91</v>
       </c>
-      <c r="C58" t="s">
-        <v>92</v>
-      </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G58">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="H58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>246</v>
+        <v>294</v>
       </c>
       <c r="B59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" t="s">
         <v>93</v>
       </c>
-      <c r="C59" t="s">
-        <v>142</v>
-      </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E59" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="G59">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="H59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="E60" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H60">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="I60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>227</v>
+        <v>361</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D61" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E61" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>230</v>
+        <v>354</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E62" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>231</v>
+        <v>343</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D63" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E63" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E64" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>285</v>
+        <v>338</v>
       </c>
       <c r="B65" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E65" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>257</v>
+        <v>336</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D66" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="E66" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>261</v>
-      </c>
-      <c r="B67" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" t="s">
-        <v>106</v>
-      </c>
-      <c r="D67" t="s">
-        <v>134</v>
-      </c>
-      <c r="E67" t="s">
-        <v>134</v>
-      </c>
-      <c r="F67">
-        <f t="shared" ref="F67:F81" si="4">COUNTIF(D67:E67, "S")</f>
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <f t="shared" ref="G67:G81" si="5">COUNTIF(D67:E67, "P")</f>
-        <v>2</v>
-      </c>
-      <c r="H67">
-        <f t="shared" ref="H67:H81" si="6">COUNTIF(D67:E67, "N")</f>
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <f t="shared" ref="I67:I81" si="7">SUM(F67:H67)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>262</v>
-      </c>
-      <c r="B68" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" t="s">
-        <v>108</v>
-      </c>
-      <c r="D68" t="s">
-        <v>134</v>
-      </c>
-      <c r="E68" t="s">
-        <v>134</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>307</v>
-      </c>
-      <c r="B69" t="s">
-        <v>109</v>
-      </c>
-      <c r="C69" t="s">
-        <v>110</v>
-      </c>
-      <c r="D69" t="s">
-        <v>134</v>
-      </c>
-      <c r="E69" t="s">
-        <v>134</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>310</v>
-      </c>
-      <c r="B70" t="s">
-        <v>111</v>
-      </c>
-      <c r="C70" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" t="s">
-        <v>133</v>
-      </c>
-      <c r="E70" t="s">
-        <v>133</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>314</v>
-      </c>
-      <c r="B71" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" t="s">
-        <v>114</v>
-      </c>
-      <c r="D71" t="s">
-        <v>134</v>
-      </c>
-      <c r="E71" t="s">
-        <v>134</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>293</v>
-      </c>
-      <c r="B72" t="s">
-        <v>158</v>
-      </c>
-      <c r="C72" t="s">
-        <v>56</v>
-      </c>
-      <c r="D72" t="s">
-        <v>133</v>
-      </c>
-      <c r="E72" t="s">
-        <v>133</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G72">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>294</v>
-      </c>
-      <c r="B73" t="s">
-        <v>115</v>
-      </c>
-      <c r="C73" t="s">
-        <v>116</v>
-      </c>
-      <c r="D73" t="s">
-        <v>133</v>
-      </c>
-      <c r="E73" t="s">
-        <v>134</v>
-      </c>
-      <c r="F73">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G73">
+      <c r="G66">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H73">
+      <c r="H66">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I73">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>291</v>
-      </c>
-      <c r="B74" t="s">
-        <v>162</v>
-      </c>
-      <c r="C74" t="s">
-        <v>58</v>
-      </c>
-      <c r="D74" t="s">
-        <v>135</v>
-      </c>
-      <c r="E74" t="s">
-        <v>135</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="I74">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>361</v>
-      </c>
-      <c r="B75" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" t="s">
-        <v>133</v>
-      </c>
-      <c r="E75" t="s">
-        <v>133</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I75">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>362</v>
-      </c>
-      <c r="B76" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" t="s">
-        <v>133</v>
-      </c>
-      <c r="E76" t="s">
-        <v>133</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I76">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>354</v>
-      </c>
-      <c r="B77" t="s">
-        <v>121</v>
-      </c>
-      <c r="C77" t="s">
-        <v>122</v>
-      </c>
-      <c r="D77" t="s">
-        <v>133</v>
-      </c>
-      <c r="E77" t="s">
-        <v>133</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>343</v>
-      </c>
-      <c r="B78" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" t="s">
-        <v>123</v>
-      </c>
-      <c r="D78" t="s">
-        <v>133</v>
-      </c>
-      <c r="E78" t="s">
-        <v>133</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>321</v>
-      </c>
-      <c r="B79" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" t="s">
-        <v>133</v>
-      </c>
-      <c r="E79" t="s">
-        <v>133</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>338</v>
-      </c>
-      <c r="B80" t="s">
-        <v>126</v>
-      </c>
-      <c r="C80" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" t="s">
-        <v>133</v>
-      </c>
-      <c r="E80" t="s">
-        <v>133</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G80">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I80">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>336</v>
-      </c>
-      <c r="B81" t="s">
-        <v>128</v>
-      </c>
-      <c r="C81" t="s">
-        <v>129</v>
-      </c>
-      <c r="D81" t="s">
-        <v>133</v>
-      </c>
-      <c r="E81" t="s">
-        <v>134</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I81">
+      <c r="I66">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
@@ -3570,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A4061B-5F27-9747-8005-1F4A527B596F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3581,47 +2999,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B1">
-        <f>COUNTIF(Sheet1!F2:F81, 2)/80</f>
-        <v>0.73750000000000004</v>
+        <f>COUNTIF(Sheet1!F2:F66, 2)/65</f>
+        <v>0.72307692307692306</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(Sheet1!F2:F81, 1)/80</f>
-        <v>6.25E-2</v>
+        <f>COUNTIF(Sheet1!F2:F66, 1)/65</f>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(Sheet1!G2:G81, 2)/80</f>
-        <v>0.16250000000000001</v>
+        <f>COUNTIF(Sheet1!G2:G66, 2)/65</f>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(Sheet1!H2:H81, 1)/80</f>
+        <f>COUNTIF(Sheet1!H2:H66, 1)/65</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(Sheet1!H2:H81, 2)/80</f>
-        <v>3.7499999999999999E-2</v>
+        <f>COUNTIF(Sheet1!H2:H66, 2)/65</f>
+        <v>4.6153846153846156E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>